<commit_message>
feat: improve tool look
</commit_message>
<xml_diff>
--- a/exampleControlSheets/Performance Analysis/PerformanceAnalysisGraph.xlsx
+++ b/exampleControlSheets/Performance Analysis/PerformanceAnalysisGraph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\Documents\School\Masters\DylanLeveille\WebToolCSAT\exampleControlSheets\Performance Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191C601E-F24F-48C2-8ADB-EC8C466F9D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25E6A7C-BEE6-4BEE-8C6C-A3648F9247D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="17460" windowHeight="10260" xr2:uid="{57C133EE-0927-4076-B0D1-BEC84C99647A}"/>
   </bookViews>
@@ -288,7 +288,7 @@
                   <c:v>289</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3689</c:v>
+                  <c:v>4038</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1519,7 +1519,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1577,7 +1577,7 @@
         <v>50</v>
       </c>
       <c r="B7">
-        <v>3689</v>
+        <v>4038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>